<commit_message>
feature two commit two
</commit_message>
<xml_diff>
--- a/src/test/resources/Input.xlsx
+++ b/src/test/resources/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91948\git\Team17_Testing_Squad\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDBE3E04-A0AB-463A-B2D2-B653C03238D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD1369CF-C8D4-4D14-8A4D-4BB85CCEF9DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Name</t>
   </si>
@@ -64,13 +64,22 @@
   </si>
   <si>
     <t>Apr</t>
+  </si>
+  <si>
+    <t>Hackathon Apr Update</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>learning</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -93,6 +102,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF495057"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -130,7 +145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -147,6 +162,7 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,16 +443,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -501,6 +517,28 @@
       </c>
       <c r="C6" s="4"/>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>